<commit_message>
Added elimination Excel list for PCOS.
</commit_message>
<xml_diff>
--- a/src/test/resources/EliminatedInputData/Eliminatelist.xlsx
+++ b/src/test/resources/EliminatedInputData/Eliminatelist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viru\git\Team_15-Recipe-Hunters\src\test\resources\EliminatedInputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpalan570\Desktop\Team_15-Recipe-Hunters\src\test\resources\EliminatedInputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FFA1BB-69FB-43E5-82A4-63A31F1B9D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356EFD33-7935-4105-B230-17EB17EAB666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9BD2DDA2-3D46-4F6D-810E-6F52C06F624D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9BD2DDA2-3D46-4F6D-810E-6F52C06F624D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
-  <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
-    <t>rice</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>food category</t>
   </si>
@@ -217,13 +211,94 @@
   </si>
   <si>
     <t>peanuts</t>
+  </si>
+  <si>
+    <t>PCOS</t>
+  </si>
+  <si>
+    <t>cakes</t>
+  </si>
+  <si>
+    <t>pastries</t>
+  </si>
+  <si>
+    <t>white bread</t>
+  </si>
+  <si>
+    <t>fried food</t>
+  </si>
+  <si>
+    <t>pizza</t>
+  </si>
+  <si>
+    <t>burger</t>
+  </si>
+  <si>
+    <t>carbonated beverages</t>
+  </si>
+  <si>
+    <t>sweets</t>
+  </si>
+  <si>
+    <t>icecreams</t>
+  </si>
+  <si>
+    <t>soda</t>
+  </si>
+  <si>
+    <t>juices</t>
+  </si>
+  <si>
+    <t>red meat</t>
+  </si>
+  <si>
+    <t>dairy</t>
+  </si>
+  <si>
+    <t>soy products</t>
+  </si>
+  <si>
+    <t>gluten</t>
+  </si>
+  <si>
+    <t>pasta</t>
+  </si>
+  <si>
+    <t>white rice</t>
+  </si>
+  <si>
+    <t>doughnuts</t>
+  </si>
+  <si>
+    <t>fries</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>vegetable oil</t>
+  </si>
+  <si>
+    <t>sybean oil</t>
+  </si>
+  <si>
+    <t>canola oil</t>
+  </si>
+  <si>
+    <t>rapeseed oil</t>
+  </si>
+  <si>
+    <t>sunflower oil</t>
+  </si>
+  <si>
+    <t>safflower oil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +318,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -299,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -308,6 +390,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,245 +705,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98E75B4-1237-4A41-B364-49F3856B9C26}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="A4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="6" spans="1:7" ht="15" thickBot="1">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1">
+      <c r="A7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1">
+      <c r="A8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1">
+      <c r="A9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1">
+      <c r="A12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1">
+      <c r="A13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1">
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
-      <c r="C14" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" t="s">
-        <v>44</v>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>